<commit_message>
fix xls/xlsx so they read the row|column defaults
</commit_message>
<xml_diff>
--- a/test/style.xlsx
+++ b/test/style.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Bold</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>Italic-Underline</t>
+  </si>
+  <si>
+    <t>Bolded Row</t>
+  </si>
+  <si>
+    <t>Bolded Column</t>
+  </si>
+  <si>
+    <t>Bolded Row Italic Column</t>
   </si>
 </sst>
 </file>
@@ -425,50 +434,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1">
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>